<commit_message>
Promo paq 10k y 20k
</commit_message>
<xml_diff>
--- a/public/assets/Planilla.xlsx
+++ b/public/assets/Planilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ComoVamos\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5003B27B-0A20-4401-B5FD-D35D83493AD3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451FBE59-6C43-44B6-A25F-76FC4DCC31F5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31920" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>CIRCUITO</t>
   </si>
@@ -116,6 +116,10 @@
   </si>
   <si>
     <t>TOTAL: $ ________________</t>
+  </si>
+  <si>
+    <t>Promo Lineas Ingresadas 29, 30 y 31 de Mayo:
+Paq 10k: 3.000 • Paq 20k: $4.000</t>
   </si>
 </sst>
 </file>
@@ -423,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -438,9 +442,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -481,6 +482,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -493,7 +495,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1067,8 +1068,8 @@
   </sheetPr>
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,37 +1086,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="H2"/>
       <c r="K2"/>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="15"/>
+      <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="G3"/>
       <c r="H3"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="15" t="s">
+      <c r="K3" s="13"/>
+      <c r="L3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="15"/>
+      <c r="M3" s="14"/>
     </row>
     <row r="4" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="K4" s="14"/>
-      <c r="L4" s="15" t="s">
+      <c r="K4" s="13"/>
+      <c r="L4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="15"/>
-    </row>
-    <row r="5" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M4" s="14"/>
+    </row>
+    <row r="5" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>18</v>
       </c>
@@ -1124,34 +1125,36 @@
       <c r="D5" s="29"/>
       <c r="E5" s="29"/>
       <c r="F5" s="29"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-    </row>
-    <row r="6" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G5" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+    </row>
+    <row r="6" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29"/>
       <c r="B6" s="29"/>
       <c r="C6" s="29"/>
       <c r="D6" s="29"/>
       <c r="E6" s="29"/>
       <c r="F6" s="29"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
@@ -1193,34 +1196,34 @@
       <c r="F8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="K8" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L8" s="20" t="s">
+      <c r="L8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="22" t="s">
+      <c r="N8" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="O8" s="20" t="s">
+      <c r="O8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="P8" s="23" t="s">
+      <c r="P8" s="22" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1231,66 +1234,66 @@
       <c r="D9" s="5"/>
       <c r="E9" s="9"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="28"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="27"/>
       <c r="N9" s="10"/>
       <c r="O9" s="8"/>
       <c r="P9" s="7"/>
     </row>
     <row r="10" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
     </row>
     <row r="12" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
-      <c r="P12" s="33"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
     </row>
     <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
@@ -1299,69 +1302,69 @@
       <c r="E13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="33"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
     </row>
     <row r="14" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="14" t="s">
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="N14" s="33"/>
-      <c r="O14" s="33"/>
-      <c r="P14" s="33"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
     </row>
     <row r="15" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33"/>
-      <c r="P15" s="33"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
     </row>
     <row r="16" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D16" s="3"/>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
     </row>
     <row r="17" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D17" s="3"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
@@ -1369,13 +1372,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A5:F6"/>
     <mergeCell ref="G7:M7"/>
     <mergeCell ref="N7:O7"/>
+    <mergeCell ref="G5:P6"/>
   </mergeCells>
   <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="0.55118110236220474" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="64" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Negrita"&amp;14Fecha: ____________________________________</oddHeader>
   </headerFooter>

</xml_diff>

<commit_message>
Arreglo en planilla para promo paq 10k y 20k
</commit_message>
<xml_diff>
--- a/public/assets/Planilla.xlsx
+++ b/public/assets/Planilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ComoVamos\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451FBE59-6C43-44B6-A25F-76FC4DCC31F5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6B1762-D34C-43C2-AF3F-BB6145FBDC7F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31920" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planilla" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Planilla!$A$1:$P$18</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Planilla!$A$1:$P$19</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>CIRCUITO</t>
   </si>
@@ -120,6 +120,12 @@
   <si>
     <t>Promo Lineas Ingresadas 29, 30 y 31 de Mayo:
 Paq 10k: 3.000 • Paq 20k: $4.000</t>
+  </si>
+  <si>
+    <t>_____ x $3.000 = ________________</t>
+  </si>
+  <si>
+    <t>_____ x $4.000 = ________________</t>
   </si>
 </sst>
 </file>
@@ -1066,10 +1072,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,7 +1251,7 @@
       <c r="O9" s="8"/>
       <c r="P9" s="7"/>
     </row>
-    <row r="10" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
@@ -1263,28 +1269,25 @@
       <c r="O10" s="15"/>
       <c r="P10" s="15"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
+    <row r="11" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
     </row>
     <row r="12" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G12" s="13" t="s">
-        <v>25</v>
-      </c>
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
@@ -1296,80 +1299,87 @@
       <c r="P12" s="28"/>
     </row>
     <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="13"/>
+      <c r="B13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="G13" s="13" t="s">
+        <v>26</v>
+      </c>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
       <c r="K13" s="28"/>
       <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
       <c r="N13" s="28"/>
       <c r="O13" s="28"/>
       <c r="P13" s="28"/>
     </row>
-    <row r="14" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="G14" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
       <c r="K14" s="28"/>
       <c r="L14" s="28"/>
-      <c r="M14" s="13" t="s">
-        <v>28</v>
-      </c>
+      <c r="M14" s="28"/>
       <c r="N14" s="28"/>
       <c r="O14" s="28"/>
       <c r="P14" s="28"/>
     </row>
-    <row r="15" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
+    <row r="15" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
       <c r="K15" s="28"/>
       <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
+      <c r="M15" s="13" t="s">
+        <v>28</v>
+      </c>
       <c r="N15" s="28"/>
       <c r="O15" s="28"/>
       <c r="P15" s="28"/>
     </row>
-    <row r="16" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D16" s="3"/>
-      <c r="G16" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-    </row>
-    <row r="17" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D17" s="3"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
+      <c r="G17" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="13"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+    <row r="18" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D18" s="3"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="G19" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Mostrar Segmentado los paquetes en el total de la planilla generada.
</commit_message>
<xml_diff>
--- a/public/assets/Planilla.xlsx
+++ b/public/assets/Planilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ComoVamos\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6B1762-D34C-43C2-AF3F-BB6145FBDC7F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A94636-835D-4E55-A508-6E667659220F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31920" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Planilla" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Planilla!$A$1:$P$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Planilla!$A$1:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>CIRCUITO</t>
   </si>
@@ -84,10 +84,6 @@
     <t>Minut.</t>
   </si>
   <si>
-    <t>PLANILLA GROSS - INCENTIVO POR (PAQ 4k) DE $1.000 - (PAQ 6k y 10k) DE $1.500
-(BOLSAS-MIN-PAQUETE MAYORES $14.900) DE $2.000</t>
-  </si>
-  <si>
     <t>CALL CENTER AMCOM S.A.</t>
   </si>
   <si>
@@ -106,33 +102,22 @@
     <t>Asesor:________________________________________</t>
   </si>
   <si>
-    <t>_____ x $1.000 = ________________</t>
-  </si>
-  <si>
-    <t>_____ x $1.500 = ________________</t>
-  </si>
-  <si>
-    <t>_____ x $2.000 = ________________</t>
-  </si>
-  <si>
     <t>TOTAL: $ ________________</t>
   </si>
   <si>
     <t>Promo Lineas Ingresadas 29, 30 y 31 de Mayo:
-Paq 10k: 3.000 • Paq 20k: $4.000</t>
-  </si>
-  <si>
-    <t>_____ x $3.000 = ________________</t>
-  </si>
-  <si>
-    <t>_____ x $4.000 = ________________</t>
+Paq 10k: 3.000 • Paq 20k: $5.000</t>
+  </si>
+  <si>
+    <t>PLANILLA GROSS - INCENTIVO POR (PAQ 4k) DE $1.000 - (PAQ 6k) DE $2.000
+(BOLSAS-MIN-PAQUETE MAYORES $10.000) DE $3.000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +170,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -451,7 +442,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -489,17 +479,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -528,8 +521,8 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1381125</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>180976</xdr:rowOff>
     </xdr:to>
@@ -582,7 +575,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>274864</xdr:colOff>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>229961</xdr:rowOff>
     </xdr:from>
@@ -620,8 +613,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12036878" y="420461"/>
-          <a:ext cx="266699" cy="269420"/>
+          <a:off x="11182350" y="229961"/>
+          <a:ext cx="274863" cy="268059"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -643,7 +636,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>333454</xdr:colOff>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
@@ -688,8 +681,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12095468" y="715735"/>
-          <a:ext cx="142267" cy="229962"/>
+          <a:off x="11258550" y="523874"/>
+          <a:ext cx="170921" cy="229962"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1072,10 +1065,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A5" sqref="A5:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,7 +1076,8 @@
     <col min="1" max="1" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="29.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="24" style="1" customWidth="1"/>
     <col min="7" max="13" width="7.5703125" style="1" customWidth="1"/>
     <col min="14" max="15" width="6.7109375" style="1" customWidth="1"/>
@@ -1093,7 +1087,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K1" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L1" s="13"/>
       <c r="M1" s="13"/>
@@ -1102,7 +1096,7 @@
       <c r="H2"/>
       <c r="K2"/>
       <c r="L2" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M2" s="14"/>
     </row>
@@ -1111,56 +1105,56 @@
       <c r="H3"/>
       <c r="K3" s="13"/>
       <c r="L3" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M3" s="14"/>
     </row>
     <row r="4" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="K4" s="13"/>
       <c r="L4" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M4" s="14"/>
     </row>
     <row r="5" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
+      <c r="A5" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
     </row>
     <row r="6" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
@@ -1169,19 +1163,19 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="30" t="s">
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="32"/>
+      <c r="O7" s="31"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1202,34 +1196,34 @@
       <c r="F8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="18" t="s">
+      <c r="J8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="17" t="s">
+      <c r="K8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L8" s="19" t="s">
+      <c r="L8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="20" t="s">
+      <c r="M8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="N8" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="O8" s="19" t="s">
+      <c r="O8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="P8" s="22" t="s">
+      <c r="P8" s="21" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1240,111 +1234,94 @@
       <c r="D9" s="5"/>
       <c r="E9" s="9"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="27"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="26"/>
       <c r="N9" s="10"/>
       <c r="O9" s="8"/>
       <c r="P9" s="7"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
+    <row r="10" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
     </row>
     <row r="11" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G11" s="13" t="s">
-        <v>25</v>
-      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
     </row>
     <row r="12" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="B12" s="3"/>
+      <c r="E12" s="3"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
     </row>
     <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="G13" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
-    </row>
-    <row r="14" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
-    </row>
-    <row r="15" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+    </row>
+    <row r="14" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="3"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
+    </row>
+    <row r="15" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>27</v>
-      </c>
+      <c r="G15" s="13"/>
       <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
     </row>
     <row r="16" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D16" s="3"/>
@@ -1353,33 +1330,12 @@
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
     </row>
-    <row r="17" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D17" s="3"/>
-      <c r="G17" s="13" t="s">
-        <v>30</v>
-      </c>
+    <row r="17" spans="7:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G17" s="13"/>
       <c r="H17" s="13"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-    </row>
-    <row r="18" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D18" s="3"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-    </row>
-    <row r="19" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="28"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1389,7 +1345,7 @@
     <mergeCell ref="G5:P6"/>
   </mergeCells>
   <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="0.55118110236220474" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="65" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Negrita"&amp;14Fecha: ____________________________________</oddHeader>
   </headerFooter>

</xml_diff>

<commit_message>
Ambos estilos en total de planilla.
</commit_message>
<xml_diff>
--- a/public/assets/Planilla.xlsx
+++ b/public/assets/Planilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ComoVamos\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52C4F09-7B50-4577-BE32-3513822EB36A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EFF86A-820C-4009-BBBC-43FFAA6E0A0C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31920" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,7 +117,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,13 +164,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color rgb="FF000000"/>
@@ -424,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -439,7 +432,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -478,8 +470,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1065,10 +1056,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,75 +1077,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="H2"/>
       <c r="K2"/>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="14"/>
+      <c r="M2" s="13"/>
     </row>
     <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="G3"/>
       <c r="H3"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="14" t="s">
+      <c r="K3" s="12"/>
+      <c r="L3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="14"/>
+      <c r="M3" s="13"/>
     </row>
     <row r="4" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="K4" s="13"/>
-      <c r="L4" s="14" t="s">
+      <c r="K4" s="12"/>
+      <c r="L4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="14"/>
+      <c r="M4" s="13"/>
     </row>
     <row r="5" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="32" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
     </row>
     <row r="6" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
@@ -1163,19 +1154,19 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="29" t="s">
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="O7" s="31"/>
+      <c r="O7" s="29"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1196,34 +1187,34 @@
       <c r="F8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="16" t="s">
+      <c r="K8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="18" t="s">
+      <c r="L8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="19" t="s">
+      <c r="M8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="20" t="s">
+      <c r="N8" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="O8" s="18" t="s">
+      <c r="O8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="P8" s="21" t="s">
+      <c r="P8" s="20" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1234,94 +1225,104 @@
       <c r="D9" s="5"/>
       <c r="E9" s="9"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="26"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="25"/>
       <c r="N9" s="10"/>
       <c r="O9" s="8"/>
       <c r="P9" s="7"/>
     </row>
     <row r="10" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
     </row>
     <row r="11" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="13" t="s">
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
     </row>
     <row r="12" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
     </row>
     <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="E13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="13"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
     </row>
     <row r="14" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D14" s="3"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
     </row>
     <row r="15" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="3"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
     </row>
     <row r="16" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D16" s="3"/>
@@ -1329,13 +1330,72 @@
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="7:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="27"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+    </row>
+    <row r="17" spans="7:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+    </row>
+    <row r="18" spans="7:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+    </row>
+    <row r="19" spans="7:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+    </row>
+    <row r="20" spans="7:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+    </row>
+    <row r="21" spans="7:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Ajuste precios de paquetes para el més de Julio
</commit_message>
<xml_diff>
--- a/public/assets/Planilla.xlsx
+++ b/public/assets/Planilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ComoVamos\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B88BDBA-6510-48D0-84F2-84817D719CEB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BAFBBF-F1E0-4FCE-9B49-5CD573B60F3E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31920" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>CIRCUITO</t>
   </si>
@@ -99,11 +99,18 @@
     <t>TOTAL: $ ________________</t>
   </si>
   <si>
-    <t>PLANILLA GROSS - INCENTIVO POR (PAQ 4k) DE $1.000 - (PAQ 6k) DE $2.000
-(BOLSAS-MIN-PAQUETE MAYORES $10.000) DE $3.000</t>
-  </si>
-  <si>
     <t>FECHA PAQUETE</t>
+  </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLANILLA GROSS - INCENTIVO POR (PAQ 4k) DE $1.000 - (PAQ 6k) DE $1.500
+(BOLSAS-MIN-PAQUETE MAYORES $10.000) DE $3.000 - (PAQ 20k) DE $4.000 </t>
+  </si>
+  <si>
+    <t>PROMO: Mes Junio 29 y 30
+INCENTIVO POR (PAQ 6k) (PAQ 10k) (PAQ 20k) DE $4.000</t>
   </si>
 </sst>
 </file>
@@ -411,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -424,7 +431,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1071,73 +1077,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="H2"/>
       <c r="K2"/>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="13"/>
+      <c r="M2" s="12"/>
     </row>
     <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="G3"/>
       <c r="H3"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="13" t="s">
+      <c r="K3" s="11"/>
+      <c r="L3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="13"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="K4" s="12"/>
-      <c r="L4" s="13" t="s">
+      <c r="K4" s="11"/>
+      <c r="L4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="13"/>
+      <c r="M4" s="12"/>
     </row>
     <row r="5" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
+      <c r="A5" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
     </row>
     <row r="6" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
@@ -1146,19 +1154,19 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="27" t="s">
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="O7" s="29"/>
+      <c r="O7" s="28"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1176,37 +1184,37 @@
       <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="14" t="s">
+      <c r="F8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="16" t="s">
+      <c r="J8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="17" t="s">
+      <c r="L8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="18" t="s">
+      <c r="M8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="19" t="s">
+      <c r="N8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="O8" s="17" t="s">
+      <c r="O8" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="P8" s="20" t="s">
+      <c r="P8" s="19" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1217,177 +1225,179 @@
       <c r="D9" s="5"/>
       <c r="E9" s="9"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="10"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="O9" s="8"/>
       <c r="P9" s="7"/>
     </row>
     <row r="10" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
     </row>
     <row r="11" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12" t="s">
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
     </row>
     <row r="12" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
     </row>
     <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="E13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
     </row>
     <row r="14" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D14" s="3"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
     </row>
     <row r="15" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="3"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
     </row>
     <row r="16" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D16" s="3"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
     </row>
     <row r="17" spans="7:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
     </row>
     <row r="18" spans="7:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
     </row>
     <row r="19" spans="7:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
     </row>
     <row r="20" spans="7:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
     </row>
     <row r="21" spans="7:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>